<commit_message>
更新excel template 及40010 prod_type欄位
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/40013.xlsx
+++ b/PhoenixCI/Excel_Template/40013.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\需求單\保證金第二階段\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2. 風管組業務\B. 資訊需求單\20190502 盤後系統需求\3. 調整template\報表\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18900" windowHeight="7935"/>
+    <workbookView xWindow="238" yWindow="50" windowWidth="18895" windowHeight="7939" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rpt_future" sheetId="10" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">rpt_future!$A$1:$J$50</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">fut_3index!$A:$B</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <r>
       <rPr>
@@ -992,76 +992,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>資料日期：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2014</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>年</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>月</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>24</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>日</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>結算保證金占契約總值比例</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1206,7 +1136,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">2 </t>
+      <t xml:space="preserve">3 </t>
     </r>
     <r>
       <rPr>
@@ -1457,10 +1387,11 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="10"/>
-      <name val="細明體"/>
-      <family val="3"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1520,14 +1451,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="35" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1784,28 +1718,35 @@
     <xf numFmtId="177" fontId="34" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="34" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="34" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="34" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="25" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="29" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
     <cellStyle name="百分比 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2177,28 +2118,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.7"/>
   <cols>
-    <col min="1" max="1" width="6.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="19" style="9" customWidth="1"/>
-    <col min="4" max="4" width="21.25" style="9" customWidth="1"/>
-    <col min="5" max="5" width="18.625" style="9" customWidth="1"/>
-    <col min="6" max="7" width="19.75" style="9" customWidth="1"/>
-    <col min="8" max="8" width="19.75" style="32" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="32" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="32" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="9" customWidth="1"/>
+    <col min="6" max="7" width="19.77734375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="32" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" style="32" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="32" customWidth="1"/>
     <col min="11" max="11" width="11" style="32" customWidth="1"/>
-    <col min="12" max="13" width="9.75" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.77734375" style="32" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="32"/>
     <col min="15" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="43.9" customHeight="1">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="43.85" customHeight="1">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -2212,15 +2153,13 @@
       <c r="G1" s="97"/>
       <c r="H1" s="97"/>
       <c r="I1" s="42"/>
-      <c r="J1" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="94"/>
       <c r="L1" s="33"/>
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
     </row>
-    <row r="2" spans="1:15" s="6" customFormat="1" ht="39">
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="36.35">
       <c r="A2" s="5"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -2235,13 +2174,13 @@
         <v>5</v>
       </c>
       <c r="F2" s="91" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="91" t="s">
+      <c r="H2" s="91" t="s">
         <v>58</v>
-      </c>
-      <c r="H2" s="91" t="s">
-        <v>59</v>
       </c>
       <c r="I2" s="46"/>
       <c r="J2" s="46"/>
@@ -2251,7 +2190,7 @@
       <c r="N2" s="34"/>
       <c r="O2" s="34"/>
     </row>
-    <row r="3" spans="1:15" ht="30" customHeight="1">
+    <row r="3" spans="1:15" ht="30.05" customHeight="1">
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
@@ -2277,7 +2216,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="5" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B5" s="47"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -2292,7 +2231,7 @@
       <c r="M5" s="36"/>
       <c r="N5" s="36"/>
     </row>
-    <row r="6" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="6" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B6" s="47"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2307,7 +2246,7 @@
       <c r="M6" s="36"/>
       <c r="N6" s="36"/>
     </row>
-    <row r="7" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="7" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B7" s="47"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -2322,7 +2261,7 @@
       <c r="M7" s="36"/>
       <c r="N7" s="36"/>
     </row>
-    <row r="8" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="8" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B8" s="47"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -2337,7 +2276,7 @@
       <c r="M8" s="36"/>
       <c r="N8" s="36"/>
     </row>
-    <row r="9" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="9" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B9" s="47"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -2352,7 +2291,7 @@
       <c r="M9" s="36"/>
       <c r="N9" s="36"/>
     </row>
-    <row r="10" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="10" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B10" s="47"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -2367,7 +2306,7 @@
       <c r="M10" s="36"/>
       <c r="N10" s="36"/>
     </row>
-    <row r="11" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="11" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B11" s="47"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -2382,7 +2321,7 @@
       <c r="M11" s="36"/>
       <c r="N11" s="36"/>
     </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="12" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B12" s="47"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -2397,7 +2336,7 @@
       <c r="M12" s="36"/>
       <c r="N12" s="36"/>
     </row>
-    <row r="13" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="13" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B13" s="47"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -2412,7 +2351,7 @@
       <c r="M13" s="36"/>
       <c r="N13" s="36"/>
     </row>
-    <row r="14" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="14" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B14" s="47"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -2427,7 +2366,7 @@
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
     </row>
-    <row r="15" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="15" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B15" s="47"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -2442,7 +2381,7 @@
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
     </row>
-    <row r="16" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="16" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B16" s="47"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -2457,7 +2396,7 @@
       <c r="M16" s="36"/>
       <c r="N16" s="36"/>
     </row>
-    <row r="17" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="17" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B17" s="47"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -2472,7 +2411,7 @@
       <c r="M17" s="36"/>
       <c r="N17" s="36"/>
     </row>
-    <row r="18" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="18" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B18" s="47"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -2487,7 +2426,7 @@
       <c r="M18" s="36"/>
       <c r="N18" s="36"/>
     </row>
-    <row r="19" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="19" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B19" s="47"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -2502,7 +2441,7 @@
       <c r="M19" s="36"/>
       <c r="N19" s="36"/>
     </row>
-    <row r="20" spans="1:15" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="20" spans="1:15" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B20" s="47"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2517,12 +2456,12 @@
       <c r="M20" s="36"/>
       <c r="N20" s="36"/>
     </row>
-    <row r="21" spans="1:15" s="19" customFormat="1" ht="43.5" customHeight="1">
+    <row r="21" spans="1:15" s="19" customFormat="1" ht="43.55" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -2537,7 +2476,7 @@
       <c r="M21" s="38"/>
       <c r="N21" s="38"/>
     </row>
-    <row r="22" spans="1:15" ht="26.25" customHeight="1">
+    <row r="22" spans="1:15" ht="26.3" customHeight="1">
       <c r="B22" s="90" t="s">
         <v>49</v>
       </c>
@@ -2548,7 +2487,7 @@
       <c r="G22" s="18"/>
       <c r="H22" s="39"/>
     </row>
-    <row r="23" spans="1:15" ht="39">
+    <row r="23" spans="1:15" ht="36.35">
       <c r="B23" s="43" t="s">
         <v>2</v>
       </c>
@@ -2556,7 +2495,7 @@
         <v>51</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>8</v>
@@ -2568,7 +2507,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I23" s="92" t="s">
         <v>54</v>
@@ -2590,14 +2529,14 @@
       <c r="G24" s="21"/>
       <c r="H24" s="48"/>
       <c r="I24" s="93"/>
-      <c r="J24" s="99"/>
+      <c r="J24" s="96"/>
       <c r="K24" s="40"/>
       <c r="L24" s="40"/>
       <c r="M24" s="40"/>
       <c r="N24" s="40"/>
       <c r="O24" s="40"/>
     </row>
-    <row r="25" spans="1:15" s="14" customFormat="1" ht="18.75">
+    <row r="25" spans="1:15" s="14" customFormat="1" ht="17.55">
       <c r="B25" s="47"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2606,13 +2545,15 @@
       <c r="G25" s="9"/>
       <c r="H25" s="36"/>
       <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
+      <c r="J25" s="37">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="K25" s="37"/>
       <c r="L25" s="37"/>
       <c r="M25" s="36"/>
       <c r="N25" s="36"/>
     </row>
-    <row r="26" spans="1:15" s="14" customFormat="1" ht="22.5" hidden="1" customHeight="1">
+    <row r="26" spans="1:15" s="14" customFormat="1" ht="22.55" customHeight="1">
       <c r="B26" s="90" t="s">
         <v>50</v>
       </c>
@@ -2623,13 +2564,15 @@
       <c r="G26" s="9"/>
       <c r="H26" s="36"/>
       <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
+      <c r="J26" s="37">
+        <v>0.31</v>
+      </c>
       <c r="K26" s="37"/>
       <c r="L26" s="37"/>
       <c r="M26" s="36"/>
       <c r="N26" s="36"/>
     </row>
-    <row r="27" spans="1:15" s="14" customFormat="1" ht="36.4" hidden="1" customHeight="1">
+    <row r="27" spans="1:15" s="14" customFormat="1" ht="36.5" customHeight="1">
       <c r="B27" s="80" t="s">
         <v>2</v>
       </c>
@@ -2637,7 +2580,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>8</v>
@@ -2649,7 +2592,7 @@
         <v>10</v>
       </c>
       <c r="H27" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I27" s="92" t="s">
         <v>54</v>
@@ -2662,7 +2605,7 @@
       <c r="M27" s="36"/>
       <c r="N27" s="36"/>
     </row>
-    <row r="28" spans="1:15" s="14" customFormat="1" ht="31.9" hidden="1" customHeight="1">
+    <row r="28" spans="1:15" s="14" customFormat="1" ht="31.95" customHeight="1">
       <c r="B28" s="8" t="s">
         <v>7</v>
       </c>
@@ -2673,13 +2616,13 @@
       <c r="G28" s="21"/>
       <c r="H28" s="48"/>
       <c r="I28" s="93"/>
-      <c r="J28" s="94"/>
+      <c r="J28" s="96"/>
       <c r="K28" s="37"/>
       <c r="L28" s="37"/>
       <c r="M28" s="36"/>
       <c r="N28" s="36"/>
     </row>
-    <row r="29" spans="1:15" s="14" customFormat="1" ht="18.75">
+    <row r="29" spans="1:15" s="14" customFormat="1" ht="17.55">
       <c r="B29" s="47"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -2694,9 +2637,9 @@
       <c r="M29" s="36"/>
       <c r="N29" s="36"/>
     </row>
-    <row r="30" spans="1:15" s="14" customFormat="1" ht="21">
+    <row r="30" spans="1:15" s="14" customFormat="1" ht="22.55">
       <c r="B30" s="90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -2711,7 +2654,7 @@
       <c r="M30" s="36"/>
       <c r="N30" s="36"/>
     </row>
-    <row r="31" spans="1:15" s="14" customFormat="1" ht="39">
+    <row r="31" spans="1:15" s="14" customFormat="1" ht="36.35">
       <c r="B31" s="80" t="s">
         <v>2</v>
       </c>
@@ -2719,7 +2662,7 @@
         <v>51</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>8</v>
@@ -2731,7 +2674,7 @@
         <v>10</v>
       </c>
       <c r="H31" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I31" s="92" t="s">
         <v>54</v>
@@ -2744,7 +2687,7 @@
       <c r="M31" s="36"/>
       <c r="N31" s="36"/>
     </row>
-    <row r="32" spans="1:15" s="14" customFormat="1" ht="31.9" customHeight="1">
+    <row r="32" spans="1:15" s="14" customFormat="1" ht="31.95" customHeight="1">
       <c r="B32" s="8" t="s">
         <v>7</v>
       </c>
@@ -2755,13 +2698,13 @@
       <c r="G32" s="21"/>
       <c r="H32" s="48"/>
       <c r="I32" s="93"/>
-      <c r="J32" s="99"/>
+      <c r="J32" s="96"/>
       <c r="K32" s="37"/>
       <c r="L32" s="37"/>
       <c r="M32" s="36"/>
       <c r="N32" s="36"/>
     </row>
-    <row r="33" spans="1:18" s="14" customFormat="1" ht="18.75">
+    <row r="33" spans="1:18" s="14" customFormat="1" ht="17.55">
       <c r="B33" s="47"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -2776,7 +2719,7 @@
       <c r="M33" s="36"/>
       <c r="N33" s="36"/>
     </row>
-    <row r="34" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="34" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B34" s="47"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2791,7 +2734,7 @@
       <c r="M34" s="36"/>
       <c r="N34" s="36"/>
     </row>
-    <row r="35" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="35" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B35" s="47"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2806,7 +2749,7 @@
       <c r="M35" s="36"/>
       <c r="N35" s="36"/>
     </row>
-    <row r="36" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="36" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B36" s="47"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -2821,7 +2764,7 @@
       <c r="M36" s="36"/>
       <c r="N36" s="36"/>
     </row>
-    <row r="37" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="37" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B37" s="47"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -2836,7 +2779,7 @@
       <c r="M37" s="36"/>
       <c r="N37" s="36"/>
     </row>
-    <row r="38" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="38" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B38" s="47"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -2851,7 +2794,7 @@
       <c r="M38" s="36"/>
       <c r="N38" s="36"/>
     </row>
-    <row r="39" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="39" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B39" s="47"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -2866,7 +2809,7 @@
       <c r="M39" s="36"/>
       <c r="N39" s="36"/>
     </row>
-    <row r="40" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="40" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B40" s="47"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -2881,7 +2824,7 @@
       <c r="M40" s="36"/>
       <c r="N40" s="36"/>
     </row>
-    <row r="41" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="41" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B41" s="47"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -2896,7 +2839,7 @@
       <c r="M41" s="36"/>
       <c r="N41" s="36"/>
     </row>
-    <row r="42" spans="1:18" s="14" customFormat="1" ht="18.75" hidden="1">
+    <row r="42" spans="1:18" s="14" customFormat="1" ht="17.55" hidden="1">
       <c r="B42" s="47"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
@@ -2911,7 +2854,7 @@
       <c r="M42" s="36"/>
       <c r="N42" s="36"/>
     </row>
-    <row r="43" spans="1:18" ht="26.25" customHeight="1">
+    <row r="43" spans="1:18" ht="26.3" customHeight="1">
       <c r="A43" s="56" t="s">
         <v>48</v>
       </c>
@@ -2935,7 +2878,7 @@
       <c r="Q43" s="54"/>
       <c r="R43" s="54"/>
     </row>
-    <row r="44" spans="1:18" ht="26.25" customHeight="1">
+    <row r="44" spans="1:18" ht="26.3" customHeight="1">
       <c r="A44" s="56"/>
       <c r="B44" s="49"/>
       <c r="C44" s="24"/>
@@ -2974,12 +2917,12 @@
       <c r="Q45" s="54"/>
       <c r="R45" s="54"/>
     </row>
-    <row r="46" spans="1:18" ht="19.5">
+    <row r="46" spans="1:18" ht="18.2">
       <c r="A46" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="89" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="26"/>
       <c r="D46" s="15"/>
@@ -3010,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="89" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D48" s="27"/>
       <c r="E48" s="4"/>
@@ -3052,32 +2995,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="T1" sqref="T1:T1048576"/>
       <selection pane="topRight" activeCell="T1" sqref="T1:T1048576"/>
       <selection pane="bottomLeft" activeCell="T1" sqref="T1:T1048576"/>
-      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomRight" activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18.2"/>
   <cols>
     <col min="1" max="1" width="11" style="58" customWidth="1"/>
-    <col min="2" max="2" width="16.125" style="58" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="58" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="58" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="58" customWidth="1"/>
-    <col min="6" max="17" width="10.25" style="58" customWidth="1"/>
-    <col min="18" max="19" width="11.875" style="58" customWidth="1"/>
-    <col min="20" max="20" width="10.25" style="58" customWidth="1"/>
-    <col min="21" max="23" width="10.5" style="76" customWidth="1"/>
-    <col min="24" max="24" width="11.125" style="76" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="58" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" style="58" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="58" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="58" customWidth="1"/>
+    <col min="6" max="17" width="10.21875" style="58" customWidth="1"/>
+    <col min="18" max="18" width="11.88671875" style="58" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" style="99" customWidth="1"/>
+    <col min="20" max="20" width="10.21875" style="58" customWidth="1"/>
+    <col min="21" max="23" width="10.44140625" style="76" customWidth="1"/>
+    <col min="24" max="24" width="11.109375" style="76" customWidth="1"/>
     <col min="25" max="27" width="11" style="77" customWidth="1"/>
-    <col min="28" max="31" width="11.125" style="76" customWidth="1"/>
-    <col min="32" max="33" width="9.375" style="78" customWidth="1"/>
-    <col min="34" max="34" width="11.125" style="78" customWidth="1"/>
-    <col min="35" max="37" width="11.125" style="79" customWidth="1"/>
-    <col min="38" max="16384" width="8.875" style="58"/>
+    <col min="28" max="31" width="11.109375" style="76" customWidth="1"/>
+    <col min="32" max="33" width="9.33203125" style="78" customWidth="1"/>
+    <col min="34" max="34" width="11.109375" style="78" customWidth="1"/>
+    <col min="35" max="37" width="11.109375" style="79" customWidth="1"/>
+    <col min="38" max="16384" width="8.88671875" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="42.75" customHeight="1">
@@ -3105,7 +3049,7 @@
       <c r="AJ1" s="98"/>
       <c r="AK1" s="98"/>
     </row>
-    <row r="2" spans="1:37" ht="78">
+    <row r="2" spans="1:37" ht="73.25">
       <c r="A2" s="81" t="s">
         <v>16</v>
       </c>
@@ -3160,7 +3104,7 @@
       <c r="R2" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="82" t="s">
+      <c r="S2" s="100" t="s">
         <v>33</v>
       </c>
       <c r="T2" s="83" t="s">
@@ -3237,7 +3181,7 @@
       <c r="P3" s="68"/>
       <c r="Q3" s="68"/>
       <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
+      <c r="S3" s="101"/>
       <c r="T3" s="69"/>
       <c r="U3" s="72"/>
       <c r="V3" s="73"/>
@@ -3276,7 +3220,7 @@
       <c r="P4" s="68"/>
       <c r="Q4" s="68"/>
       <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
+      <c r="S4" s="101"/>
       <c r="T4" s="69"/>
       <c r="U4" s="72"/>
       <c r="V4" s="73"/>
@@ -3315,7 +3259,7 @@
       <c r="P5" s="68"/>
       <c r="Q5" s="68"/>
       <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
+      <c r="S5" s="101"/>
       <c r="T5" s="69"/>
       <c r="U5" s="72"/>
       <c r="V5" s="73"/>
@@ -3354,7 +3298,7 @@
       <c r="P6" s="68"/>
       <c r="Q6" s="68"/>
       <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
+      <c r="S6" s="101"/>
       <c r="T6" s="69"/>
       <c r="U6" s="72"/>
       <c r="V6" s="73"/>
@@ -3393,7 +3337,7 @@
       <c r="P7" s="68"/>
       <c r="Q7" s="68"/>
       <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
+      <c r="S7" s="101"/>
       <c r="T7" s="69"/>
       <c r="U7" s="72"/>
       <c r="V7" s="73"/>
@@ -3432,7 +3376,7 @@
       <c r="P8" s="68"/>
       <c r="Q8" s="68"/>
       <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
+      <c r="S8" s="101"/>
       <c r="T8" s="69"/>
       <c r="U8" s="72"/>
       <c r="V8" s="73"/>
@@ -3471,7 +3415,7 @@
       <c r="P9" s="68"/>
       <c r="Q9" s="68"/>
       <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
+      <c r="S9" s="101"/>
       <c r="T9" s="69"/>
       <c r="U9" s="72"/>
       <c r="V9" s="73"/>
@@ -3510,7 +3454,7 @@
       <c r="P10" s="68"/>
       <c r="Q10" s="68"/>
       <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
+      <c r="S10" s="101"/>
       <c r="T10" s="69"/>
       <c r="U10" s="72"/>
       <c r="V10" s="73"/>
@@ -3549,7 +3493,7 @@
       <c r="P11" s="68"/>
       <c r="Q11" s="68"/>
       <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
+      <c r="S11" s="101"/>
       <c r="T11" s="69"/>
       <c r="U11" s="72"/>
       <c r="V11" s="73"/>
@@ -3588,7 +3532,7 @@
       <c r="P12" s="68"/>
       <c r="Q12" s="68"/>
       <c r="R12" s="62"/>
-      <c r="S12" s="62"/>
+      <c r="S12" s="101"/>
       <c r="T12" s="69"/>
       <c r="U12" s="72"/>
       <c r="V12" s="73"/>
@@ -3627,7 +3571,7 @@
       <c r="P13" s="68"/>
       <c r="Q13" s="68"/>
       <c r="R13" s="62"/>
-      <c r="S13" s="62"/>
+      <c r="S13" s="101"/>
       <c r="T13" s="69"/>
       <c r="U13" s="72"/>
       <c r="V13" s="73"/>
@@ -3666,7 +3610,7 @@
       <c r="P14" s="68"/>
       <c r="Q14" s="68"/>
       <c r="R14" s="62"/>
-      <c r="S14" s="62"/>
+      <c r="S14" s="101"/>
       <c r="T14" s="69"/>
       <c r="U14" s="72"/>
       <c r="V14" s="73"/>
@@ -3705,7 +3649,7 @@
       <c r="P15" s="68"/>
       <c r="Q15" s="68"/>
       <c r="R15" s="62"/>
-      <c r="S15" s="62"/>
+      <c r="S15" s="101"/>
       <c r="T15" s="69"/>
       <c r="U15" s="72"/>
       <c r="V15" s="73"/>
@@ -3744,7 +3688,7 @@
       <c r="P16" s="68"/>
       <c r="Q16" s="68"/>
       <c r="R16" s="62"/>
-      <c r="S16" s="62"/>
+      <c r="S16" s="101"/>
       <c r="T16" s="69"/>
       <c r="U16" s="72"/>
       <c r="V16" s="73"/>
@@ -3783,7 +3727,7 @@
       <c r="P17" s="68"/>
       <c r="Q17" s="68"/>
       <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
+      <c r="S17" s="101"/>
       <c r="T17" s="69"/>
       <c r="U17" s="72"/>
       <c r="V17" s="73"/>
@@ -3822,7 +3766,7 @@
       <c r="P18" s="68"/>
       <c r="Q18" s="68"/>
       <c r="R18" s="62"/>
-      <c r="S18" s="62"/>
+      <c r="S18" s="101"/>
       <c r="T18" s="69"/>
       <c r="U18" s="72"/>
       <c r="V18" s="73"/>
@@ -3861,7 +3805,7 @@
       <c r="P19" s="68"/>
       <c r="Q19" s="68"/>
       <c r="R19" s="62"/>
-      <c r="S19" s="62"/>
+      <c r="S19" s="101"/>
       <c r="T19" s="69"/>
       <c r="U19" s="72"/>
       <c r="V19" s="73"/>
@@ -3900,7 +3844,7 @@
       <c r="P20" s="68"/>
       <c r="Q20" s="68"/>
       <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
+      <c r="S20" s="101"/>
       <c r="T20" s="69"/>
       <c r="U20" s="72"/>
       <c r="V20" s="73"/>
@@ -3939,7 +3883,7 @@
       <c r="P21" s="68"/>
       <c r="Q21" s="68"/>
       <c r="R21" s="62"/>
-      <c r="S21" s="62"/>
+      <c r="S21" s="101"/>
       <c r="T21" s="69"/>
       <c r="U21" s="72"/>
       <c r="V21" s="73"/>
@@ -3978,7 +3922,7 @@
       <c r="P22" s="68"/>
       <c r="Q22" s="68"/>
       <c r="R22" s="62"/>
-      <c r="S22" s="62"/>
+      <c r="S22" s="101"/>
       <c r="T22" s="69"/>
       <c r="U22" s="72"/>
       <c r="V22" s="73"/>
@@ -4017,7 +3961,7 @@
       <c r="P23" s="68"/>
       <c r="Q23" s="68"/>
       <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
+      <c r="S23" s="101"/>
       <c r="T23" s="69"/>
       <c r="U23" s="72"/>
       <c r="V23" s="73"/>
@@ -4056,7 +4000,7 @@
       <c r="P24" s="68"/>
       <c r="Q24" s="68"/>
       <c r="R24" s="62"/>
-      <c r="S24" s="62"/>
+      <c r="S24" s="101"/>
       <c r="T24" s="69"/>
       <c r="U24" s="72"/>
       <c r="V24" s="73"/>
@@ -4095,7 +4039,7 @@
       <c r="P25" s="68"/>
       <c r="Q25" s="68"/>
       <c r="R25" s="62"/>
-      <c r="S25" s="62"/>
+      <c r="S25" s="101"/>
       <c r="T25" s="69"/>
       <c r="U25" s="72"/>
       <c r="V25" s="73"/>
@@ -4134,7 +4078,7 @@
       <c r="P26" s="68"/>
       <c r="Q26" s="68"/>
       <c r="R26" s="62"/>
-      <c r="S26" s="62"/>
+      <c r="S26" s="101"/>
       <c r="T26" s="69"/>
       <c r="U26" s="72"/>
       <c r="V26" s="73"/>
@@ -4173,7 +4117,7 @@
       <c r="P27" s="68"/>
       <c r="Q27" s="68"/>
       <c r="R27" s="62"/>
-      <c r="S27" s="62"/>
+      <c r="S27" s="101"/>
       <c r="T27" s="69"/>
       <c r="U27" s="72"/>
       <c r="V27" s="73"/>
@@ -4212,7 +4156,7 @@
       <c r="P28" s="68"/>
       <c r="Q28" s="68"/>
       <c r="R28" s="62"/>
-      <c r="S28" s="62"/>
+      <c r="S28" s="101"/>
       <c r="T28" s="69"/>
       <c r="U28" s="72"/>
       <c r="V28" s="73"/>
@@ -4251,7 +4195,7 @@
       <c r="P29" s="68"/>
       <c r="Q29" s="68"/>
       <c r="R29" s="62"/>
-      <c r="S29" s="62"/>
+      <c r="S29" s="101"/>
       <c r="T29" s="69"/>
       <c r="U29" s="72"/>
       <c r="V29" s="73"/>
@@ -4290,7 +4234,7 @@
       <c r="P30" s="68"/>
       <c r="Q30" s="68"/>
       <c r="R30" s="62"/>
-      <c r="S30" s="62"/>
+      <c r="S30" s="101"/>
       <c r="T30" s="69"/>
       <c r="U30" s="72"/>
       <c r="V30" s="73"/>
@@ -4313,7 +4257,7 @@
     <row r="33" spans="2:21">
       <c r="B33" s="87"/>
     </row>
-    <row r="34" spans="2:21" ht="19.5">
+    <row r="34" spans="2:21">
       <c r="U34" s="88" t="s">
         <v>47</v>
       </c>

</xml_diff>